<commit_message>
update excel, adding keys
</commit_message>
<xml_diff>
--- a/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
+++ b/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Downloads\udacity_Joyce\Data Warehousing\peer learning\github\Redwood DM Solution\DM Solution Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B5441F-80E9-4A81-A717-F8032D8BFAA4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887602E7-9658-45E1-8B70-50F781A031D8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23020" windowHeight="9040" tabRatio="950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
   <si>
     <t>Object Name</t>
   </si>
@@ -128,30 +128,18 @@
     <t>date</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket.ListingKey</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.FactDaysOnMarket.PropertyKey</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket.ListingAgentKey</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.FactDaysOnMarket.BeginListDate</t>
   </si>
   <si>
     <t>DWRedwood.dbo.FactDaysOnMarket.EndListDate</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.Listing.ListingID</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.Listing.PropertyID</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.Listing.ListingAgentKey</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.Listing.BeginListDate</t>
   </si>
   <si>
@@ -318,6 +306,21 @@
   </si>
   <si>
     <t>DWRedwood.dbo.DimDates.YearName</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactDaysOnMarket.LocationKey</t>
+  </si>
+  <si>
+    <t>generated</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactDaysOnMarke.tAgentKey</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactDaysOnMarket.DateKey</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.Listing.ListingAgentID</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -445,7 +448,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,10 +863,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:E42"/>
+  <dimension ref="A3:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -932,7 +934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="13" customFormat="1">
+    <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
         <v>35</v>
       </c>
@@ -940,7 +942,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>10</v>
@@ -951,13 +953,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>10</v>
@@ -967,48 +969,44 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="11" t="s">
-        <v>37</v>
+      <c r="A9" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="C9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.4" customHeight="1">
+        <v>96</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>34</v>
@@ -1017,52 +1015,52 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:5" ht="14.4" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>10</v>
@@ -1070,64 +1068,64 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>10</v>
@@ -1138,13 +1136,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>10</v>
@@ -1155,166 +1153,166 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="8" t="s">
+      <c r="D25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="14.4" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>19</v>
-      </c>
       <c r="C26" s="11" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>12</v>
+      <c r="E28" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B29" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>12</v>
@@ -1325,78 +1323,78 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="9" t="s">
+      <c r="C33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>19</v>
+        <v>86</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>22</v>
@@ -1405,29 +1403,29 @@
         <v>22</v>
       </c>
       <c r="E34" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>19</v>
@@ -1439,29 +1437,29 @@
         <v>22</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="11" t="s">
+      <c r="C37" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>19</v>
@@ -1473,12 +1471,12 @@
         <v>22</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>19</v>
@@ -1490,12 +1488,12 @@
         <v>22</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>19</v>
@@ -1507,12 +1505,12 @@
         <v>22</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>19</v>
@@ -1524,23 +1522,40 @@
         <v>22</v>
       </c>
       <c r="E41" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update excel workingduration and age
</commit_message>
<xml_diff>
--- a/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
+++ b/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Downloads\udacity_Joyce\Data Warehousing\peer learning\github\Redwood DM Solution\DM Solution Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887602E7-9658-45E1-8B70-50F781A031D8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45E9688-D490-4062-836C-6CA35B1F3C21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23020" windowHeight="9040" tabRatio="950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="100">
   <si>
     <t>Object Name</t>
   </si>
@@ -239,12 +239,6 @@
     <t>DWRedwood.dbo.DimAgent.FirstName</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.DimAgent.HireDate</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimAgent.BirthDate</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.DimAgent.Gender</t>
   </si>
   <si>
@@ -321,6 +315,12 @@
   </si>
   <si>
     <t>DWRedwood.dbo.Listing.ListingAgentID</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimAgent.WorkingDuration</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimAgent.Age</t>
   </si>
 </sst>
 </file>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -953,13 +953,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>10</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>11</v>
@@ -987,16 +987,20 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+        <v>94</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
@@ -1278,13 +1282,13 @@
         <v>19</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1295,86 +1299,86 @@
         <v>19</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>13</v>
@@ -1391,7 +1395,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>11</v>
@@ -1408,7 +1412,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>19</v>
@@ -1425,7 +1429,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>19</v>
@@ -1442,7 +1446,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>19</v>
@@ -1459,7 +1463,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>19</v>
@@ -1476,7 +1480,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>19</v>
@@ -1493,7 +1497,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>19</v>
@@ -1510,7 +1514,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>19</v>
@@ -1527,7 +1531,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
update hiredate and birthdate
</commit_message>
<xml_diff>
--- a/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
+++ b/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Downloads\udacity_Joyce\Data Warehousing\peer learning\github\Redwood DM Solution\DM Solution Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45E9688-D490-4062-836C-6CA35B1F3C21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0370D953-3446-4259-9E17-38F5AB374564}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23020" windowHeight="9040" tabRatio="950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,6 +239,12 @@
     <t>DWRedwood.dbo.DimAgent.FirstName</t>
   </si>
   <si>
+    <t>DWRedwood.dbo.DimAgent.HireDate</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimAgent.BirthDate</t>
+  </si>
+  <si>
     <t>DWRedwood.dbo.DimAgent.Gender</t>
   </si>
   <si>
@@ -315,12 +321,6 @@
   </si>
   <si>
     <t>DWRedwood.dbo.Listing.ListingAgentID</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimAgent.WorkingDuration</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimAgent.Age</t>
   </si>
 </sst>
 </file>
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -953,13 +953,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>10</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>11</v>
@@ -987,13 +987,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>22</v>
@@ -1282,13 +1282,13 @@
         <v>19</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1299,86 +1299,86 @@
         <v>19</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>13</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>11</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>19</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>19</v>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>19</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>19</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>19</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>19</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>19</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated Excel Table with new IP content
</commit_message>
<xml_diff>
--- a/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
+++ b/Redwood DM Solution/DM Solution Documentation/Redwood Solution Workbook.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Downloads\udacity_Joyce\Data Warehousing\peer learning\github\Redwood DM Solution\DM Solution Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0370D953-3446-4259-9E17-38F5AB374564}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23020" windowHeight="9040" tabRatio="950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23020" windowHeight="9040" tabRatio="950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Members" sheetId="7" r:id="rId1"/>
     <sheet name="Data Warehouse" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="124">
   <si>
     <t>Object Name</t>
   </si>
@@ -86,9 +85,6 @@
     <t>nvarchar(50)</t>
   </si>
   <si>
-    <t>Generated</t>
-  </si>
-  <si>
     <t>na</t>
   </si>
   <si>
@@ -122,24 +118,9 @@
     <t>Redwood.dbo.Listing</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket.PropertyKey</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket.BeginListDate</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket.EndListDate</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.Listing.PropertyID</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.Listing.BeginListDate</t>
   </si>
   <si>
@@ -185,45 +166,9 @@
     <t>numeric(4, 2)</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.DimLocation.LocationKey</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimLocation.City</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimLocation.Zipcode</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimPropertyCharacteristics.PropetyKey</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimPropertyCharacteristics.Bedrooms</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimPropertyCharacteristics.Bathrooms</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimPropertyCharacteristics.YearBuilt</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimPropertyCharacteristics.Lotsize</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimPropertyCharacteristics.Stories</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimPropertyCharacteristics.SqFt</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.DimAgent</t>
   </si>
   <si>
-    <t xml:space="preserve">DWRedwood.dbo.DimPropertyCharacteristics </t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.DimLocation</t>
-  </si>
-  <si>
     <t>DWRedwood.dbo.Agent</t>
   </si>
   <si>
@@ -308,25 +253,151 @@
     <t>DWRedwood.dbo.DimDates.YearName</t>
   </si>
   <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket.LocationKey</t>
-  </si>
-  <si>
-    <t>generated</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.FactDaysOnMarke.tAgentKey</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.FactDaysOnMarket.DateKey</t>
-  </si>
-  <si>
-    <t>DWRedwood.dbo.Listing.ListingAgentID</t>
+    <t>DWRedwood.dbo.DimAgent.StatusText</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.Agent.StatusText</t>
+  </si>
+  <si>
+    <t>nvarchar(25)</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.PropetyKey</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.Bedrooms</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.Bathrooms</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.YearBuilt</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.Stories</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.Lotsize</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.SqFt</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.Type</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.PropetyType.Type</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.Zone</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.PropetyType.Zone</t>
+  </si>
+  <si>
+    <t>nvarchar(4)</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.Zipcode</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimProperty.City</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.SaleStatus.SaleStatus</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DmProperty.SaleStatus</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Customer</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimCustomer</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimCustomer.CustomerKey</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.Customer.CustomerID</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.CustomerType.Description</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimCustomer.CustomerTypeDescription</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimCustomer.City</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.Customer.City</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimCustomer.Zipcode</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.Customer.Zipcode</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.DimCustomer.ContactReasonDescription</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.ContactReason.Description</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.EndListDate</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.BeginListDate</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.CommissionRate</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.DateKey</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.AgentKey</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.AskingPrice</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.BidPrice</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.CustAgentList.CommisionRate</t>
+  </si>
+  <si>
+    <t>numeric(4, 4)</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.CustAgentList.BidPrice</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.Listing.AskingPrice</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.PropetyKey</t>
+  </si>
+  <si>
+    <t>DWRedwood.dbo.FactEfficiency.CustomerKey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -541,23 +612,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -593,23 +647,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -785,7 +822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -816,10 +853,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3">
         <v>8</v>
@@ -830,10 +867,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4">
         <v>8</v>
@@ -844,10 +881,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5">
         <v>8</v>
@@ -862,11 +899,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:E43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -880,7 +917,7 @@
   <sheetData>
     <row r="3" spans="1:5" ht="18.5">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -902,13 +939,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>8</v>
@@ -919,13 +956,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>7</v>
@@ -936,16 +973,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="11" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>10</v>
@@ -953,13 +990,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="11" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>10</v>
@@ -969,597 +1006,784 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="12" t="s">
-        <v>98</v>
+      <c r="A9" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="C9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="11" t="s">
-        <v>95</v>
+      <c r="A10" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="C10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="11" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>7</v>
+      <c r="A13" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="11" t="s">
-        <v>54</v>
+      <c r="A14" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
+        <v>121</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="11" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>43</v>
+      <c r="A16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>7</v>
+      <c r="A17" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>10</v>
+      <c r="A22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="11" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>7</v>
+      <c r="A25" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="11" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="14.4" customHeight="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="11" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="11" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>12</v>
+        <v>41</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="11" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>12</v>
+        <v>42</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>83</v>
+        <v>44</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>84</v>
+        <v>46</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" s="8" t="s">
+      <c r="A33" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="9" t="s">
+      <c r="C35" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>12</v>
+      <c r="E35" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>50</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="14.4" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>10</v>
+        <v>52</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>20</v>
+        <v>64</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>22</v>
+        <v>60</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>22</v>
+        <v>61</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>22</v>
+        <v>62</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>22</v>
+        <v>63</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="E42" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="6" t="s">
+    <row r="48" spans="1:5">
+      <c r="A48" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D54" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E54" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>